<commit_message>
Se agregaron campos como fecha y tema. Repoila datos correctamente hasta la página indicada
</commit_message>
<xml_diff>
--- a/info/descargas.xlsx
+++ b/info/descargas.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D146"/>
+  <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,22 +440,32 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>page</t>
+          <t>Pagina</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>card</t>
+          <t>Tarjeta</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>title</t>
+          <t>Titulo</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>process_number</t>
+          <t>Numero de proceso</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Tema</t>
         </is>
       </c>
     </row>
@@ -472,6 +486,14 @@
           <t>2015-800-77</t>
         </is>
       </c>
+      <c r="E2" s="2" t="n">
+        <v>42251</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Régimen de conflicto de intereses</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -490,6 +512,14 @@
           <t>2013-801-096</t>
         </is>
       </c>
+      <c r="E3" s="2" t="n">
+        <v>41689</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Responsabilidad de liquidadores</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -508,6 +538,14 @@
           <t>2016-800-002</t>
         </is>
       </c>
+      <c r="E4" s="2" t="n">
+        <v>42458</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -526,6 +564,14 @@
           <t>2016-800-084</t>
         </is>
       </c>
+      <c r="E5" s="2" t="n">
+        <v>43083</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Régimen de conflicto de intereses</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -544,6 +590,14 @@
           <t>2016-800-142</t>
         </is>
       </c>
+      <c r="E6" s="2" t="n">
+        <v>43171</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -562,6 +616,14 @@
           <t>2017-800-00167</t>
         </is>
       </c>
+      <c r="E7" s="2" t="n">
+        <v>43249</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Régimen de conflicto de intereses</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -580,6 +642,14 @@
           <t>2019-800-00067</t>
         </is>
       </c>
+      <c r="E8" s="2" t="n">
+        <v>43767</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -598,6 +668,14 @@
           <t>2017-800-00288</t>
         </is>
       </c>
+      <c r="E9" s="2" t="n">
+        <v>43686</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -616,6 +694,14 @@
           <t>2018-800-00455</t>
         </is>
       </c>
+      <c r="E10" s="2" t="n">
+        <v>43867</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -634,6 +720,14 @@
           <t>2019-800-00419</t>
         </is>
       </c>
+      <c r="E11" s="2" t="n">
+        <v>44235</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Responsabilidad de liquidadores</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -652,6 +746,14 @@
           <t>2020-800-00173</t>
         </is>
       </c>
+      <c r="E12" s="2" t="n">
+        <v>44245</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -670,6 +772,14 @@
           <t>2020-800-00152</t>
         </is>
       </c>
+      <c r="E13" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -688,6 +798,14 @@
           <t>2020-800-00101</t>
         </is>
       </c>
+      <c r="E14" s="2" t="n">
+        <v>44351</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -706,6 +824,14 @@
           <t>2021-800-00036</t>
         </is>
       </c>
+      <c r="E15" s="2" t="n">
+        <v>44375</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Abuso del derecho de voto</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -724,6 +850,14 @@
           <t>2012-801-029</t>
         </is>
       </c>
+      <c r="E16" s="2" t="n">
+        <v>41697</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Abuso del derecho de voto</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -742,6 +876,14 @@
           <t>2018-800-00470</t>
         </is>
       </c>
+      <c r="E17" s="2" t="n">
+        <v>43894</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Régimen de conflicto de intereses</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -760,6 +902,14 @@
           <t>2021-800-00148</t>
         </is>
       </c>
+      <c r="E18" s="2" t="n">
+        <v>44753</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Régimen de conflicto de intereses</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -778,6 +928,14 @@
           <t>2020-800-00176</t>
         </is>
       </c>
+      <c r="E19" s="2" t="n">
+        <v>44524</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Resolución de conflictos societarios</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -796,6 +954,14 @@
           <t>2020-800-00047</t>
         </is>
       </c>
+      <c r="E20" s="2" t="n">
+        <v>45540</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -814,6 +980,14 @@
           <t>2022-800-00350</t>
         </is>
       </c>
+      <c r="E21" s="2" t="n">
+        <v>45506</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Responsabilidad de liquidadores</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -832,6 +1006,14 @@
           <t>2016-800-034</t>
         </is>
       </c>
+      <c r="E22" s="2" t="n">
+        <v>42573</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -850,6 +1032,14 @@
           <t>2014-801-270</t>
         </is>
       </c>
+      <c r="E23" s="2" t="n">
+        <v>42221</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Régimen de conflicto de intereses</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -868,6 +1058,14 @@
           <t>2017-800-00185</t>
         </is>
       </c>
+      <c r="E24" s="2" t="n">
+        <v>43432</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -886,6 +1084,14 @@
           <t>2016-800-370</t>
         </is>
       </c>
+      <c r="E25" s="2" t="n">
+        <v>43389</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -904,6 +1110,14 @@
           <t>2017-800-00406</t>
         </is>
       </c>
+      <c r="E26" s="2" t="n">
+        <v>43585</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -922,6 +1136,14 @@
           <t>2016-800-181</t>
         </is>
       </c>
+      <c r="E27" s="2" t="n">
+        <v>43076</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -940,6 +1162,14 @@
           <t>2020-800-00270</t>
         </is>
       </c>
+      <c r="E28" s="2" t="n">
+        <v>44272</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Inexistencia de las decisiones sociales</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -958,6 +1188,14 @@
           <t>2022-800-00319</t>
         </is>
       </c>
+      <c r="E29" s="2" t="n">
+        <v>45070</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -976,6 +1214,14 @@
           <t>2017-800-00288</t>
         </is>
       </c>
+      <c r="E30" s="2" t="n">
+        <v>43686</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -994,6 +1240,14 @@
           <t>2018-800-00455</t>
         </is>
       </c>
+      <c r="E31" s="2" t="n">
+        <v>43867</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1012,6 +1266,14 @@
           <t>2019-800-00419</t>
         </is>
       </c>
+      <c r="E32" s="2" t="n">
+        <v>44235</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Responsabilidad de liquidadores</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1030,6 +1292,14 @@
           <t>2020-800-00173</t>
         </is>
       </c>
+      <c r="E33" s="2" t="n">
+        <v>44245</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1048,6 +1318,14 @@
           <t>2020-800-00152</t>
         </is>
       </c>
+      <c r="E34" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1066,6 +1344,14 @@
           <t>2018-800-00241</t>
         </is>
       </c>
+      <c r="E35" s="2" t="n">
+        <v>44133</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1084,6 +1370,14 @@
           <t>2021-800-00126</t>
         </is>
       </c>
+      <c r="E36" s="2" t="n">
+        <v>44705</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1094,12 +1388,20 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2018-800-00349</t>
+          <t>2020-800-00217</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>44694</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
     </row>
@@ -1112,12 +1414,20 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Ejecución específica de acuerdos de accionistas</t>
+          <t>Abuso del derecho de voto</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2020-800-00169</t>
+          <t>2018-800-00033</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>43678</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Abuso del derecho de voto</t>
         </is>
       </c>
     </row>
@@ -1130,12 +1440,20 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2014-801-022</t>
+          <t>2021-800-00458</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>44720</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
     </row>
@@ -1148,12 +1466,20 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
+          <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2014-801-208</t>
+          <t>2019-800-00199</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>44683</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
     </row>
@@ -1166,12 +1492,20 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Responsabilidad de administradores</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2018-800-00213</t>
+          <t>2020-800-00101</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>44351</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
     </row>
@@ -1184,12 +1518,20 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Resolución de conflictos societarios</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2021-800-00036</t>
+          <t>2020-800-00039</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>44111</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Resolución de conflictos societarios</t>
         </is>
       </c>
     </row>
@@ -1202,12 +1544,20 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>El Tribunal declaró la nulidad de lo actuado Abuso del derecho de voto</t>
+          <t>Resolución de conflictos societarios</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2012-801-029</t>
+          <t>2018-800-00097</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>43576</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Resolución de conflictos societarios</t>
         </is>
       </c>
     </row>
@@ -1225,7 +1575,15 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2014-801-054</t>
+          <t>2021-800-00274</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>44609</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Régimen de conflicto de intereses</t>
         </is>
       </c>
     </row>
@@ -1238,12 +1596,20 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
+          <t>Abuso del derecho al voto</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2018-800-00220</t>
+          <t>2020-800-00246</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>44617</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Abuso del derecho de voto</t>
         </is>
       </c>
     </row>
@@ -1256,12 +1622,20 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
+          <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2021-800-00043</t>
+          <t>2016-800-00394</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>43633</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
     </row>
@@ -1282,6 +1656,14 @@
           <t>2017-800-00355</t>
         </is>
       </c>
+      <c r="E47" s="2" t="n">
+        <v>43510</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Responsabilidad de liquidadores</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -1300,6 +1682,14 @@
           <t>2019-800-00270</t>
         </is>
       </c>
+      <c r="E48" s="2" t="n">
+        <v>43754</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Resolución de conflictos societarios</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -1318,6 +1708,14 @@
           <t>2019-800-00377</t>
         </is>
       </c>
+      <c r="E49" s="2" t="n">
+        <v>43986</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Abuso del derecho de voto</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -1336,6 +1734,14 @@
           <t>2018-800-00361</t>
         </is>
       </c>
+      <c r="E50" s="2" t="n">
+        <v>43747</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1354,6 +1760,14 @@
           <t>2020-800-00031</t>
         </is>
       </c>
+      <c r="E51" s="2" t="n">
+        <v>44433</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1372,6 +1786,14 @@
           <t>2020-800-00169</t>
         </is>
       </c>
+      <c r="E52" s="2" t="n">
+        <v>44419</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Ejecución específica de acuerdos de accionistas</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1390,6 +1812,14 @@
           <t>2016-800-28</t>
         </is>
       </c>
+      <c r="E53" s="2" t="n">
+        <v>43019</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Abuso del derecho de voto</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1408,6 +1838,14 @@
           <t>810-000057</t>
         </is>
       </c>
+      <c r="E54" s="2" t="n">
+        <v>43290</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1426,6 +1864,14 @@
           <t>2020-800-00124</t>
         </is>
       </c>
+      <c r="E55" s="2" t="n">
+        <v>44152</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -1444,6 +1890,14 @@
           <t>2020-800-00264</t>
         </is>
       </c>
+      <c r="E56" s="2" t="n">
+        <v>44266</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Responsabilidad de liquidadores</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -1462,6 +1916,14 @@
           <t>2015-800-88</t>
         </is>
       </c>
+      <c r="E57" s="2" t="n">
+        <v>42277</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -1480,6 +1942,14 @@
           <t>2016-800-318</t>
         </is>
       </c>
+      <c r="E58" s="2" t="n">
+        <v>43293</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -1498,6 +1968,14 @@
           <t>2015-800-267</t>
         </is>
       </c>
+      <c r="E59" s="2" t="n">
+        <v>42958</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -1516,6 +1994,14 @@
           <t>2016-800-069</t>
         </is>
       </c>
+      <c r="E60" s="2" t="n">
+        <v>42816</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -1534,6 +2020,14 @@
           <t>2017-800-00248</t>
         </is>
       </c>
+      <c r="E61" s="2" t="n">
+        <v>43521</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -1552,6 +2046,14 @@
           <t>2018-800-00017</t>
         </is>
       </c>
+      <c r="E62" s="2" t="n">
+        <v>43592</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Resolución de conflictos societarios</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -1570,6 +2072,14 @@
           <t>2019-800-00021</t>
         </is>
       </c>
+      <c r="E63" s="2" t="n">
+        <v>43735</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Abuso del derecho de voto</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -1588,6 +2098,14 @@
           <t>2018-800-00218</t>
         </is>
       </c>
+      <c r="E64" s="2" t="n">
+        <v>43588</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Inexistencia de las decisiones sociales</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -1606,6 +2124,14 @@
           <t>2015-800-302</t>
         </is>
       </c>
+      <c r="E65" s="2" t="n">
+        <v>42913</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -1624,6 +2150,14 @@
           <t>2016-800-98</t>
         </is>
       </c>
+      <c r="E66" s="2" t="n">
+        <v>42949</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Régimen de conflicto de intereses</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -1634,12 +2168,20 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Resolución de conflictos societarios</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2016-800-00394</t>
+          <t>2018-800-00236</t>
+        </is>
+      </c>
+      <c r="E67" s="2" t="n">
+        <v>43552</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Resolución de conflictos societarios</t>
         </is>
       </c>
     </row>
@@ -1652,12 +2194,20 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Responsabilidad de liquidadores</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2017-800-00355</t>
+          <t>2014-801-229</t>
+        </is>
+      </c>
+      <c r="E68" s="2" t="n">
+        <v>42297</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
     </row>
@@ -1670,12 +2220,20 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Resolución de conflictos societarios</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2019-800-00270</t>
+          <t>2014-801-260</t>
+        </is>
+      </c>
+      <c r="E69" s="2" t="n">
+        <v>42250</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
     </row>
@@ -1688,12 +2246,20 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2019-800-00377</t>
+          <t>2015-800-100</t>
+        </is>
+      </c>
+      <c r="E70" s="2" t="n">
+        <v>42284</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
     </row>
@@ -1706,12 +2272,20 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Enajenación de acciones</t>
+          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2018-800-00221</t>
+          <t>2014-801-251</t>
+        </is>
+      </c>
+      <c r="E71" s="2" t="n">
+        <v>42200</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
         </is>
       </c>
     </row>
@@ -1729,7 +2303,15 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2015-800-130</t>
+          <t>2016-800-097</t>
+        </is>
+      </c>
+      <c r="E72" s="2" t="n">
+        <v>42629</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
         </is>
       </c>
     </row>
@@ -1742,12 +2324,20 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Impugnación de decisiones sociales</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2016-800-144</t>
+          <t>2017-800-056</t>
+        </is>
+      </c>
+      <c r="E73" s="2" t="n">
+        <v>42808</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
     </row>
@@ -1760,12 +2350,20 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2015-801-4</t>
+          <t>2017-800-058</t>
+        </is>
+      </c>
+      <c r="E74" s="2" t="n">
+        <v>42808</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
     </row>
@@ -1778,12 +2376,20 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Enajenación de acciones</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2014801-089</t>
+          <t>2016-800-198</t>
+        </is>
+      </c>
+      <c r="E75" s="2" t="n">
+        <v>42832</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Enajenación de acciones</t>
         </is>
       </c>
     </row>
@@ -1796,12 +2402,20 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Resolución de conflictos societarios</t>
+          <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2013-801-028</t>
+          <t>2013-801-166</t>
+        </is>
+      </c>
+      <c r="E76" s="2" t="n">
+        <v>42781</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
     </row>
@@ -1822,6 +2436,14 @@
           <t>2015-800-266</t>
         </is>
       </c>
+      <c r="E77" s="2" t="n">
+        <v>42579</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Nulidad de los actos defraudatorios</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -1840,6 +2462,14 @@
           <t>2015-800-182</t>
         </is>
       </c>
+      <c r="E78" s="2" t="n">
+        <v>42619</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -1858,6 +2488,14 @@
           <t>2015-800-32</t>
         </is>
       </c>
+      <c r="E79" s="2" t="n">
+        <v>42762</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -1876,6 +2514,14 @@
           <t>2017-800-00282</t>
         </is>
       </c>
+      <c r="E80" s="2" t="n">
+        <v>43438</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Responsabilidad de liquidadores</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -1894,6 +2540,14 @@
           <t>2017-800-00256</t>
         </is>
       </c>
+      <c r="E81" s="2" t="n">
+        <v>43489</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -1909,7 +2563,15 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2016-800-9</t>
+          <t>2022-800-00215</t>
+        </is>
+      </c>
+      <c r="E82" s="2" t="n">
+        <v>44999</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
     </row>
@@ -1927,7 +2589,15 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2019-800-00033</t>
+          <t>2014801013</t>
+        </is>
+      </c>
+      <c r="E83" s="2" t="n">
+        <v>41754</v>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
     </row>
@@ -1940,12 +2610,20 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
+          <t>Impugnación de actos de asambleas, juntas directivas, juntas de socios o de cualquier otro órgano directivo de personas sometidas a su supervisión. Código General del Proceso artículo 24 numeral quinto letra c)</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2014-801-158</t>
+          <t>2018-800-00396</t>
+        </is>
+      </c>
+      <c r="E84" s="2" t="n">
+        <v>43626</v>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
     </row>
@@ -1958,12 +2636,20 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Impugnación de actos de asambleas, juntas directivas, juntas de socios o de cualquier otro órgano directivo de personas sometidas a su supervisión. Código General del Proceso artículo 24 numeral quinto letra c)</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2014-801-166</t>
+          <t>2016-800-196</t>
+        </is>
+      </c>
+      <c r="E85" s="2" t="n">
+        <v>42907</v>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
     </row>
@@ -1976,12 +2662,20 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
+          <t>Impugnación de actos de asambleas, juntas directivas, juntas de socios o de cualquier otro órgano directivo de personas sometidas a su supervisión. Código General del Proceso artículo 24 numeral quinto letra c)</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>810-000053</t>
+          <t>800-000034</t>
+        </is>
+      </c>
+      <c r="E86" s="2" t="n">
+        <v>41137</v>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
     </row>
@@ -1994,12 +2688,20 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
+          <t>Responsabilidad de liquidadores</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2014-801-026</t>
+          <t>2020-800-00207</t>
+        </is>
+      </c>
+      <c r="E87" s="2" t="n">
+        <v>44594</v>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Responsabilidad de liquidadores</t>
         </is>
       </c>
     </row>
@@ -2012,14 +2714,18 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Articulo 24 del codigo general del proceso</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>2015-800-128</t>
-        </is>
-      </c>
+          <t>2015-800-238</t>
+        </is>
+      </c>
+      <c r="E88" s="2" t="n">
+        <v>42362</v>
+      </c>
+      <c r="F88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -2030,14 +2736,18 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2015-800-256</t>
-        </is>
-      </c>
+          <t>2017-800-74</t>
+        </is>
+      </c>
+      <c r="E89" s="2" t="n">
+        <v>43369</v>
+      </c>
+      <c r="F89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -2048,14 +2758,14 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>2015-800-184</t>
-        </is>
-      </c>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr"/>
+      <c r="E90" s="2" t="n">
+        <v>43360</v>
+      </c>
+      <c r="F90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -2066,14 +2776,18 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>2015-800-255</t>
-        </is>
-      </c>
+          <t>2018-800-00248</t>
+        </is>
+      </c>
+      <c r="E91" s="2" t="n">
+        <v>43521</v>
+      </c>
+      <c r="F91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -2092,6 +2806,14 @@
           <t>2016-800-255</t>
         </is>
       </c>
+      <c r="E92" s="2" t="n">
+        <v>42851</v>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Responsabilidad de liquidadores</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -2110,6 +2832,14 @@
           <t>2016-800-409</t>
         </is>
       </c>
+      <c r="E93" s="2" t="n">
+        <v>42921</v>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -2128,6 +2858,14 @@
           <t>800-000060</t>
         </is>
       </c>
+      <c r="E94" s="2" t="n">
+        <v>42927</v>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -2146,6 +2884,14 @@
           <t>2015-800-239</t>
         </is>
       </c>
+      <c r="E95" s="2" t="n">
+        <v>45040</v>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -2164,6 +2910,14 @@
           <t>2016-800-174</t>
         </is>
       </c>
+      <c r="E96" s="2" t="n">
+        <v>43111</v>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -2182,6 +2936,14 @@
           <t>2017-800-00305</t>
         </is>
       </c>
+      <c r="E97" s="2" t="n">
+        <v>43445</v>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Enajenación de acciones</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -2200,6 +2962,10 @@
           <t>2022-800-00283</t>
         </is>
       </c>
+      <c r="E98" s="2" t="n">
+        <v>44970</v>
+      </c>
+      <c r="F98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -2218,6 +2984,14 @@
           <t>2015-800-084</t>
         </is>
       </c>
+      <c r="E99" s="2" t="n">
+        <v>42542</v>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Responsabilidad de liquidadores</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -2236,6 +3010,14 @@
           <t>2014-801-240</t>
         </is>
       </c>
+      <c r="E100" s="2" t="n">
+        <v>42755</v>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Abuso del derecho de voto</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -2254,6 +3036,14 @@
           <t>2018-800-00431</t>
         </is>
       </c>
+      <c r="E101" s="2" t="n">
+        <v>43705</v>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Resolución de conflictos societarios</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -2264,12 +3054,20 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Régimen de conflicto de intereses</t>
+          <t>Responsabilidad de liquidadores</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>2015-800-86</t>
+          <t>2016-800-387</t>
+        </is>
+      </c>
+      <c r="E102" s="2" t="n">
+        <v>43278</v>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Responsabilidad de liquidadores</t>
         </is>
       </c>
     </row>
@@ -2282,12 +3080,20 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Designación de peritos</t>
+          <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>2014-801-127</t>
+          <t>2020-800-00325</t>
+        </is>
+      </c>
+      <c r="E103" s="2" t="n">
+        <v>44726</v>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
     </row>
@@ -2300,12 +3106,20 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>2014-801-163</t>
+          <t>2022-800-00406</t>
+        </is>
+      </c>
+      <c r="E104" s="2" t="n">
+        <v>45343</v>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
     </row>
@@ -2323,7 +3137,15 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>2014-801-084</t>
+          <t>2022-800-00112</t>
+        </is>
+      </c>
+      <c r="E105" s="2" t="n">
+        <v>45154</v>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
     </row>
@@ -2336,12 +3158,20 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Designación de peritos</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>2014-801-129</t>
+          <t>2019-800-00314</t>
+        </is>
+      </c>
+      <c r="E106" s="2" t="n">
+        <v>43999</v>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
     </row>
@@ -2354,12 +3184,20 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>2013-801-012</t>
+          <t>2015-800-021</t>
+        </is>
+      </c>
+      <c r="E107" s="2" t="n">
+        <v>42173</v>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
     </row>
@@ -2372,12 +3210,20 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
+          <t>Designación de peritos</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>2013-801-070</t>
+          <t>2014-801-199</t>
+        </is>
+      </c>
+      <c r="E108" s="2" t="n">
+        <v>42244</v>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Designación de peritos</t>
         </is>
       </c>
     </row>
@@ -2390,12 +3236,20 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Régimen de conflicto de intereses</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>2023-800-00487</t>
+          <t>2014-801-271</t>
+        </is>
+      </c>
+      <c r="E109" s="2" t="n">
+        <v>42250</v>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
     </row>
@@ -2408,12 +3262,20 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
+          <t>Régimen de conflicto de intereses</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>2012-801-048</t>
+          <t>2017-800-109</t>
+        </is>
+      </c>
+      <c r="E110" s="2" t="n">
+        <v>43021</v>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Régimen de conflicto de intereses</t>
         </is>
       </c>
     </row>
@@ -2426,12 +3288,20 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
+          <t>Responsabilidad de liquidadores</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>2017-800-00333</t>
+          <t>2017-800-00223</t>
+        </is>
+      </c>
+      <c r="E111" s="2" t="n">
+        <v>43084</v>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Responsabilidad de liquidadores</t>
         </is>
       </c>
     </row>
@@ -2444,12 +3314,20 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Articulo 24 del codigo general del proceso</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>2016-800-232</t>
+          <t>2012-801-059</t>
+        </is>
+      </c>
+      <c r="E112" s="2" t="n">
+        <v>42650</v>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
     </row>
@@ -2462,12 +3340,20 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>2017-800-00272</t>
+          <t>2018-800-00417</t>
+        </is>
+      </c>
+      <c r="E113" s="2" t="n">
+        <v>45441</v>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
     </row>
@@ -2480,12 +3366,20 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Régimen de conflicto de intereses</t>
+          <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>2017-800-00277</t>
+          <t>2019-800-00293</t>
+        </is>
+      </c>
+      <c r="E114" s="2" t="n">
+        <v>45469</v>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
     </row>
@@ -2498,12 +3392,20 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Enajenación de acciones</t>
+          <t>Abuso del derecho de voto</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>2013-801-123</t>
+          <t>2016-800-370</t>
+        </is>
+      </c>
+      <c r="E115" s="2" t="n">
+        <v>43370</v>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Abuso del derecho de voto</t>
         </is>
       </c>
     </row>
@@ -2516,12 +3418,20 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>2013801052</t>
+          <t>2018-800-00270</t>
+        </is>
+      </c>
+      <c r="E116" s="2" t="n">
+        <v>43735</v>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
     </row>
@@ -2542,6 +3452,14 @@
           <t>2017-800-70</t>
         </is>
       </c>
+      <c r="E117" s="2" t="n">
+        <v>43200</v>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -2560,6 +3478,14 @@
           <t>2013-801-059</t>
         </is>
       </c>
+      <c r="E118" s="2" t="n">
+        <v>41514</v>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -2578,6 +3504,14 @@
           <t>801-000042</t>
         </is>
       </c>
+      <c r="E119" s="2" t="n">
+        <v>41474</v>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Designación de peritos</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -2596,6 +3530,14 @@
           <t>2014-801-177</t>
         </is>
       </c>
+      <c r="E120" s="2" t="n">
+        <v>42121</v>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Resolución de conflictos societarios</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -2614,6 +3556,14 @@
           <t>2013-802-019</t>
         </is>
       </c>
+      <c r="E121" s="2" t="n">
+        <v>42360</v>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Resolución de conflictos societarios</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -2632,6 +3582,14 @@
           <t>2014-801-50</t>
         </is>
       </c>
+      <c r="E122" s="2" t="n">
+        <v>45021</v>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Resolución de conflictos societarios</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -2650,6 +3608,14 @@
           <t>2014-801-263</t>
         </is>
       </c>
+      <c r="E123" s="2" t="n">
+        <v>42552</v>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -2668,6 +3634,14 @@
           <t>2015-800-25</t>
         </is>
       </c>
+      <c r="E124" s="2" t="n">
+        <v>42667</v>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -2686,6 +3660,14 @@
           <t>2012-801-059</t>
         </is>
       </c>
+      <c r="E125" s="2" t="n">
+        <v>42650</v>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -2704,6 +3686,14 @@
           <t>2018-800-00417</t>
         </is>
       </c>
+      <c r="E126" s="2" t="n">
+        <v>45441</v>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -2722,6 +3712,14 @@
           <t>2019-800-00293</t>
         </is>
       </c>
+      <c r="E127" s="2" t="n">
+        <v>45469</v>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Impugnación de decisiones sociales</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -2740,6 +3738,14 @@
           <t>2016-800-370</t>
         </is>
       </c>
+      <c r="E128" s="2" t="n">
+        <v>43370</v>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>Abuso del derecho de voto</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -2758,6 +3764,14 @@
           <t>2018-800-00270</t>
         </is>
       </c>
+      <c r="E129" s="2" t="n">
+        <v>43735</v>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -2776,6 +3790,14 @@
           <t>2018-800-00361</t>
         </is>
       </c>
+      <c r="E130" s="2" t="n">
+        <v>43747</v>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -2794,6 +3816,14 @@
           <t>2020-800-00031</t>
         </is>
       </c>
+      <c r="E131" s="2" t="n">
+        <v>44433</v>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -2812,6 +3842,14 @@
           <t>2011-802-001</t>
         </is>
       </c>
+      <c r="E132" s="2" t="n">
+        <v>45042</v>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -2830,6 +3868,14 @@
           <t>2023-800-00376</t>
         </is>
       </c>
+      <c r="E133" s="2" t="n">
+        <v>45447</v>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -2848,6 +3894,14 @@
           <t>800-000051</t>
         </is>
       </c>
+      <c r="E134" s="2" t="n">
+        <v>41256</v>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -2866,6 +3920,14 @@
           <t>2011-802-003</t>
         </is>
       </c>
+      <c r="E135" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -2884,6 +3946,14 @@
           <t>2015-800-056</t>
         </is>
       </c>
+      <c r="E136" s="2" t="n">
+        <v>42424</v>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Abuso del derecho de voto</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -2894,12 +3964,20 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>2015-800-88</t>
+          <t>810-000057</t>
+        </is>
+      </c>
+      <c r="E137" s="2" t="n">
+        <v>43290</v>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
     </row>
@@ -2912,12 +3990,20 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Enajenación de acciones</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>2016-800-318</t>
+          <t>2018-800-00221</t>
+        </is>
+      </c>
+      <c r="E138" s="2" t="n">
+        <v>43679</v>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Enajenación de acciones</t>
         </is>
       </c>
     </row>
@@ -2930,12 +4016,20 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>2015-800-267</t>
+          <t>2015-800-130</t>
+        </is>
+      </c>
+      <c r="E139" s="2" t="n">
+        <v>42394</v>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
         </is>
       </c>
     </row>
@@ -2948,12 +4042,20 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
+          <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>2016-800-069</t>
+          <t>2016-800-144</t>
+        </is>
+      </c>
+      <c r="E140" s="2" t="n">
+        <v>42611</v>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
     </row>
@@ -2966,12 +4068,20 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>2017-800-00248</t>
+          <t>2015-801-4</t>
+        </is>
+      </c>
+      <c r="E141" s="2" t="n">
+        <v>42135</v>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
     </row>
@@ -2984,12 +4094,20 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Resolución de conflictos societarios</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>2014801-089</t>
+          <t>2018-800-00017</t>
+        </is>
+      </c>
+      <c r="E142" s="2" t="n">
+        <v>43592</v>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Resolución de conflictos societarios</t>
         </is>
       </c>
     </row>
@@ -3002,12 +4120,20 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Resolución de conflictos societarios</t>
+          <t>Abuso del derecho de voto</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>2013-801-028</t>
+          <t>2019-800-00021</t>
+        </is>
+      </c>
+      <c r="E143" s="2" t="n">
+        <v>43735</v>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Abuso del derecho de voto</t>
         </is>
       </c>
     </row>
@@ -3020,12 +4146,20 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Régimen de conflicto de intereses</t>
+          <t>Diferencias que ocurran entre los accionistas, o entre éstos y la sociedad o entre éstos y sus administradores, en desarrollo del contrato social o del acto unilateral. Código General del Proceso artículo 24 numeral quinta letra b)</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>2018-800-00409</t>
+          <t>2018-800-00218</t>
+        </is>
+      </c>
+      <c r="E144" s="2" t="n">
+        <v>43588</v>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Inexistencia de las decisiones sociales</t>
         </is>
       </c>
     </row>
@@ -3038,12 +4172,20 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Responsabilidad de liquidadores</t>
+          <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>2018-800-00316</t>
+          <t>2015-800-302</t>
+        </is>
+      </c>
+      <c r="E145" s="2" t="n">
+        <v>42913</v>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
     </row>
@@ -3056,12 +4198,150 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
+          <t>Régimen de conflicto de intereses</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>2016-800-98</t>
+        </is>
+      </c>
+      <c r="E146" s="2" t="n">
+        <v>42949</v>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Régimen de conflicto de intereses</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>30</v>
+      </c>
+      <c r="B147" t="n">
+        <v>1</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
           <t>Impugnación de actos de asambleas, juntas directivas, juntas de socios o de cualquier otro órgano directivo de personas sometidas a su supervisión. Código General del Proceso artículo 24 numeral quinto letra c)</t>
         </is>
       </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>2019-800-00391</t>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>2016-800-239</t>
+        </is>
+      </c>
+      <c r="E147" s="2" t="n">
+        <v>42894</v>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Impugnación de decisiones sociales</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>30</v>
+      </c>
+      <c r="B148" t="n">
+        <v>2</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Impugnación de actos de asambleas, juntas directivas, juntas de socios o de cualquier otro órgano directivo de personas sometidas a su supervisión. Código General del Proceso artículo 24 numeral quinto letra c)</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>2014-801-096</t>
+        </is>
+      </c>
+      <c r="E148" s="2" t="n">
+        <v>41907</v>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Impugnación de decisiones sociales</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>30</v>
+      </c>
+      <c r="B149" t="n">
+        <v>3</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Impugnación de actos de asambleas, juntas directivas, juntas de socios o de cualquier otro órgano directivo de personas sometidas a su supervisión. Código General del Proceso artículo 24 numeral quinto letra c)</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>2013-801-055</t>
+        </is>
+      </c>
+      <c r="E149" s="2" t="n">
+        <v>41612</v>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Impugnación de decisiones sociales</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>30</v>
+      </c>
+      <c r="B150" t="n">
+        <v>4</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Impugnación de actos de asambleas, juntas directivas, juntas de socios o de cualquier otro órgano directivo de personas sometidas a su supervisión. Código General del Proceso artículo 24 numeral quinto letra c)</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>800-000034</t>
+        </is>
+      </c>
+      <c r="E150" s="2" t="n">
+        <v>41137</v>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Impugnación de decisiones sociales</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>30</v>
+      </c>
+      <c r="B151" t="n">
+        <v>5</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Impugnación de actos de asambleas, juntas directivas, juntas de socios o de cualquier otro órgano directivo de personas sometidas a su supervisión. Código General del Proceso artículo 24 numeral quinto letra c)</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>2013-801-113</t>
+        </is>
+      </c>
+      <c r="E151" s="2" t="n">
+        <v>41824</v>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ahora se agregó el número de radicado respectivo
</commit_message>
<xml_diff>
--- a/info/descargas.xlsx
+++ b/info/descargas.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F151"/>
+  <dimension ref="A1:G151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,32 +440,37 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Pagina</t>
+          <t>page</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Tarjeta</t>
+          <t>card</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Titulo</t>
+          <t>title</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Numero de proceso</t>
+          <t>process_number</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Fecha</t>
+          <t>date</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Tema</t>
+          <t>theme</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>numero_radicado</t>
         </is>
       </c>
     </row>
@@ -494,6 +499,11 @@
           <t>Régimen de conflicto de intereses</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2015-01-368272</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -520,6 +530,11 @@
           <t>Responsabilidad de liquidadores</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2015-01-049664</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -546,6 +561,11 @@
           <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2016-01-118080</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -572,6 +592,11 @@
           <t>Régimen de conflicto de intereses</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2017-01-635814</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -598,6 +623,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2018-01-088633</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -624,6 +654,11 @@
           <t>Régimen de conflicto de intereses</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2018-01-270859</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -650,6 +685,11 @@
           <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2019-01-393233</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -660,20 +700,25 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2017-800-00288</t>
+          <t>2017-800-00158</t>
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>43686</v>
+        <v>43318</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2018-01-360173</t>
         </is>
       </c>
     </row>
@@ -691,15 +736,20 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2018-800-00455</t>
+          <t>2017-800-00234</t>
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>43867</v>
+        <v>43119</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2018-01-013074</t>
         </is>
       </c>
     </row>
@@ -712,20 +762,25 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Responsabilidad de liquidadores</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2019-800-00419</t>
+          <t>2015-800-34</t>
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>44235</v>
+        <v>43161</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Responsabilidad de liquidadores</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2018-01-076748</t>
         </is>
       </c>
     </row>
@@ -743,15 +798,20 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2020-800-00173</t>
+          <t>2015-800-303</t>
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>44245</v>
+        <v>42863</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
           <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2017-01-246764</t>
         </is>
       </c>
     </row>
@@ -764,20 +824,25 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Diferencias que ocurran entre los accionistas, o entre éstos y la sociedad o entre éstos y sus administradores, en desarrollo del contrato social o del acto unilateral. Código General del Proceso artículo 24 numeral quinta letra b)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2020-800-00152</t>
+          <t>2016-800-171</t>
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>44257</v>
+        <v>42690</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Inexistencia de las decisiones sociales</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2016-01-551771</t>
         </is>
       </c>
     </row>
@@ -795,15 +860,20 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2020-800-00101</t>
+          <t>2013-801-134</t>
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>44351</v>
+        <v>41596</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2013-01-450179</t>
         </is>
       </c>
     </row>
@@ -816,20 +886,25 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Diferencias que ocurran entre los accionistas, o entre éstos y la sociedad o entre éstos y sus administradores, en desarrollo del contrato social o del acto unilateral. Código General del Proceso artículo 24 numeral quinta letra b)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2021-800-00036</t>
+          <t>2021-800-00052</t>
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>44375</v>
+        <v>45056</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Inexistencia de las decisiones sociales</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2023-01-422361</t>
         </is>
       </c>
     </row>
@@ -842,20 +917,25 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>El Tribunal declaró la nulidad de lo actuado Abuso del derecho de voto</t>
+          <t>Responsabilidad de liquidadores</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2012-801-029</t>
+          <t>2018-800-00316</t>
         </is>
       </c>
       <c r="E16" s="2" t="n">
-        <v>41697</v>
+        <v>43802</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Responsabilidad de liquidadores</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2019-01-431266</t>
         </is>
       </c>
     </row>
@@ -873,15 +953,20 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2018-800-00470</t>
+          <t>2014-801-054</t>
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>43894</v>
+        <v>41883</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
           <t>Régimen de conflicto de intereses</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2014-01-389500</t>
         </is>
       </c>
     </row>
@@ -894,20 +979,25 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Régimen de conflicto de intereses</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2021-800-00148</t>
+          <t>2016-800-034</t>
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>44753</v>
+        <v>42573</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Régimen de conflicto de intereses</t>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2016-01-389129</t>
         </is>
       </c>
     </row>
@@ -920,20 +1010,25 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Resolución de conflictos societarios</t>
+          <t>Régimen de conflicto de intereses</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2020-800-00176</t>
+          <t>2014-801-270</t>
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>44524</v>
+        <v>42221</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Resolución de conflictos societarios</t>
+          <t>Régimen de conflicto de intereses</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2015-01-341328</t>
         </is>
       </c>
     </row>
@@ -951,15 +1046,20 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2020-800-00047</t>
+          <t>2017-800-00185</t>
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>45540</v>
+        <v>43432</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
           <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2018-01-504337</t>
         </is>
       </c>
     </row>
@@ -972,20 +1072,25 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Responsabilidad de liquidadores</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2022-800-00350</t>
+          <t>2016-800-370</t>
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>45506</v>
+        <v>43389</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Responsabilidad de liquidadores</t>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2018-01-453711</t>
         </is>
       </c>
     </row>
@@ -1003,15 +1108,20 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2016-800-034</t>
+          <t>2017-800-00406</t>
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>42573</v>
+        <v>43585</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
           <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2019-01-175241</t>
         </is>
       </c>
     </row>
@@ -1024,20 +1134,25 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Régimen de conflicto de intereses</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2014-801-270</t>
+          <t>2016-800-181</t>
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>42221</v>
+        <v>43076</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Régimen de conflicto de intereses</t>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2017-01-630134</t>
         </is>
       </c>
     </row>
@@ -1050,20 +1165,25 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Régimen de conflicto de intereses</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2017-800-00185</t>
+          <t>2018-800-00470</t>
         </is>
       </c>
       <c r="E24" s="2" t="n">
-        <v>43432</v>
+        <v>43894</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Régimen de conflicto de intereses</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2020-01-092778</t>
         </is>
       </c>
     </row>
@@ -1076,20 +1196,25 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Régimen de conflicto de intereses</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2016-800-370</t>
+          <t>2021-800-00148</t>
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>43389</v>
+        <v>44753</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Régimen de conflicto de intereses</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2022-01-555341</t>
         </is>
       </c>
     </row>
@@ -1102,20 +1227,25 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Resolución de conflictos societarios</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2017-800-00406</t>
+          <t>2020-800-00176</t>
         </is>
       </c>
       <c r="E26" s="2" t="n">
-        <v>43585</v>
+        <v>44524</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Resolución de conflictos societarios</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2021-01-692753</t>
         </is>
       </c>
     </row>
@@ -1144,6 +1274,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2017-01-630134</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1170,6 +1305,11 @@
           <t>Inexistencia de las decisiones sociales</t>
         </is>
       </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2021-01-083635</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1196,6 +1336,11 @@
           <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2023-01-460266</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1222,6 +1367,11 @@
           <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2019-01-301633</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1248,6 +1398,11 @@
           <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2020-01-038326</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1274,6 +1429,11 @@
           <t>Responsabilidad de liquidadores</t>
         </is>
       </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2021-01-028401</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1300,6 +1460,11 @@
           <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2021-01-041046</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1326,6 +1491,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>2021-01-060960</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1352,6 +1522,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2020-01-572909</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1378,6 +1553,11 @@
           <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2022-01-461652</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1388,20 +1568,25 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2020-800-00217</t>
+          <t>2018-800-00349</t>
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>44694</v>
+        <v>44300</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2021-01-132433</t>
         </is>
       </c>
     </row>
@@ -1414,20 +1599,25 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Ejecución específica de acuerdos de accionistas</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2018-800-00033</t>
+          <t>2020-800-00169</t>
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>43678</v>
+        <v>44419</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Ejecución específica de acuerdos de accionistas</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2021-01-504014</t>
         </is>
       </c>
     </row>
@@ -1440,20 +1630,25 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2021-800-00458</t>
+          <t>2014-801-022</t>
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>44720</v>
+        <v>42090</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2015-01-102274</t>
         </is>
       </c>
     </row>
@@ -1466,20 +1661,25 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Impugnación de decisiones sociales</t>
+          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2019-800-00199</t>
+          <t>2014-801-208</t>
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>44683</v>
+        <v>42066</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Impugnación de decisiones sociales</t>
+          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2015-01-061379</t>
         </is>
       </c>
     </row>
@@ -1492,20 +1692,25 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
+          <t>Responsabilidad de administradores</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2020-800-00101</t>
+          <t>2018-800-00213</t>
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>44351</v>
+        <v>43860</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Reconocimiento de presupuestos de ineficacia</t>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>2020-01-029552</t>
         </is>
       </c>
     </row>
@@ -1534,6 +1739,11 @@
           <t>Resolución de conflictos societarios</t>
         </is>
       </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>2020-01-536768</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -1560,6 +1770,11 @@
           <t>Resolución de conflictos societarios</t>
         </is>
       </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>2019-01-144180</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1586,6 +1801,11 @@
           <t>Régimen de conflicto de intereses</t>
         </is>
       </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>2022-01-073593</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1612,6 +1832,11 @@
           <t>Abuso del derecho de voto</t>
         </is>
       </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>2022-01-095075</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1638,6 +1863,11 @@
           <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2019-01-245455</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -1648,20 +1878,25 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Responsabilidad de liquidadores</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2017-800-00355</t>
+          <t>2022-800-00342</t>
         </is>
       </c>
       <c r="E47" s="2" t="n">
-        <v>43510</v>
+        <v>45121</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Responsabilidad de liquidadores</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2023-01-581550</t>
         </is>
       </c>
     </row>
@@ -1674,20 +1909,25 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Resolución de conflictos societarios</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2019-800-00270</t>
+          <t>2021-800-00377</t>
         </is>
       </c>
       <c r="E48" s="2" t="n">
-        <v>43754</v>
+        <v>44813</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Resolución de conflictos societarios</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>2022-01-672076</t>
         </is>
       </c>
     </row>
@@ -1700,20 +1940,25 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2019-800-00377</t>
+          <t>2019-800-00316</t>
         </is>
       </c>
       <c r="E49" s="2" t="n">
-        <v>43986</v>
+        <v>44035</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>2020-01-354197</t>
         </is>
       </c>
     </row>
@@ -1726,20 +1971,25 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Abuso de derecho de voto</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2018-800-00361</t>
+          <t>2019-800-00224</t>
         </is>
       </c>
       <c r="E50" s="2" t="n">
-        <v>43747</v>
+        <v>44096</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Abuso del derecho de voto</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>2020-01-519467</t>
         </is>
       </c>
     </row>
@@ -1752,20 +2002,25 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2020-800-00031</t>
+          <t>2018-800-00349</t>
         </is>
       </c>
       <c r="E51" s="2" t="n">
-        <v>44433</v>
+        <v>44300</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>2021-01-132433</t>
         </is>
       </c>
     </row>
@@ -1794,6 +2049,11 @@
           <t>Ejecución específica de acuerdos de accionistas</t>
         </is>
       </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2021-01-504014</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1820,6 +2080,11 @@
           <t>Abuso del derecho de voto</t>
         </is>
       </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>2017-01-526491</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1846,6 +2111,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2018-01-314262</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1872,6 +2142,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>2020-01-600712</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -1898,6 +2173,11 @@
           <t>Responsabilidad de liquidadores</t>
         </is>
       </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>2021-01-075199</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -1924,6 +2204,11 @@
           <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
         </is>
       </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>2015-01-398811</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -1950,6 +2235,11 @@
           <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>2018-01-320178</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -1976,6 +2266,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>2017-01-426087</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2002,6 +2297,11 @@
           <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>2017-01-121577</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -2028,6 +2328,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>2019-01-042088</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2038,20 +2343,25 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Resolución de conflictos societarios</t>
+          <t>Responsabilidad de administradores</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2018-800-00017</t>
+          <t>2018-800-00213</t>
         </is>
       </c>
       <c r="E62" s="2" t="n">
-        <v>43592</v>
+        <v>43860</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Resolución de conflictos societarios</t>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>2020-01-029552</t>
         </is>
       </c>
     </row>
@@ -2064,20 +2374,25 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Resolución de conflictos societarios</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2019-800-00021</t>
+          <t>2020-800-00039</t>
         </is>
       </c>
       <c r="E63" s="2" t="n">
-        <v>43735</v>
+        <v>44111</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Resolución de conflictos societarios</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>2020-01-536768</t>
         </is>
       </c>
     </row>
@@ -2090,20 +2405,25 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Diferencias que ocurran entre los accionistas, o entre éstos y la sociedad o entre éstos y sus administradores, en desarrollo del contrato social o del acto unilateral. Código General del Proceso artículo 24 numeral quinta letra b)</t>
+          <t>Resolución de conflictos societarios</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2018-800-00218</t>
+          <t>2018-800-00097</t>
         </is>
       </c>
       <c r="E64" s="2" t="n">
-        <v>43588</v>
+        <v>43576</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Inexistencia de las decisiones sociales</t>
+          <t>Resolución de conflictos societarios</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>2019-01-144180</t>
         </is>
       </c>
     </row>
@@ -2116,20 +2436,25 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Régimen de conflicto de intereses</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2015-800-302</t>
+          <t>2021-800-00274</t>
         </is>
       </c>
       <c r="E65" s="2" t="n">
-        <v>42913</v>
+        <v>44609</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Régimen de conflicto de intereses</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>2022-01-073593</t>
         </is>
       </c>
     </row>
@@ -2142,20 +2467,25 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Régimen de conflicto de intereses</t>
+          <t>Abuso del derecho al voto</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2016-800-98</t>
+          <t>2020-800-00246</t>
         </is>
       </c>
       <c r="E66" s="2" t="n">
-        <v>42949</v>
+        <v>44617</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Régimen de conflicto de intereses</t>
+          <t>Abuso del derecho de voto</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>2022-01-095075</t>
         </is>
       </c>
     </row>
@@ -2184,6 +2514,11 @@
           <t>Resolución de conflictos societarios</t>
         </is>
       </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>2019-01-082308</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -2210,6 +2545,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>2015-01-420775</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -2236,6 +2576,11 @@
           <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>2015-01-368166</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -2262,6 +2607,11 @@
           <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>2015-01-405304</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -2288,6 +2638,11 @@
           <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
         </is>
       </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>2015-01-320483</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -2303,15 +2658,20 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2016-800-097</t>
+          <t>2015-800-130</t>
         </is>
       </c>
       <c r="E72" s="2" t="n">
-        <v>42629</v>
+        <v>42394</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
           <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>2016-01-014398</t>
         </is>
       </c>
     </row>
@@ -2324,20 +2684,25 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
+          <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2017-800-056</t>
+          <t>2016-800-144</t>
         </is>
       </c>
       <c r="E73" s="2" t="n">
-        <v>42808</v>
+        <v>42611</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Reconocimiento de presupuestos de ineficacia</t>
+          <t>Impugnación de decisiones sociales</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>2016-01-434221</t>
         </is>
       </c>
     </row>
@@ -2350,20 +2715,25 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
+          <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2017-800-058</t>
+          <t>2015-801-4</t>
         </is>
       </c>
       <c r="E74" s="2" t="n">
-        <v>42808</v>
+        <v>42135</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Reconocimiento de presupuestos de ineficacia</t>
+          <t>Desestimación de la personalidad jurídica</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>2015-01-240134</t>
         </is>
       </c>
     </row>
@@ -2376,20 +2746,25 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Enajenación de acciones</t>
+          <t>Abuso del derecho de voto</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2016-800-198</t>
+          <t>2014801-089</t>
         </is>
       </c>
       <c r="E75" s="2" t="n">
-        <v>42832</v>
+        <v>41915</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Enajenación de acciones</t>
+          <t>Abuso del derecho de voto</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>2014-01-452112</t>
         </is>
       </c>
     </row>
@@ -2402,20 +2777,25 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Resolución de conflictos societarios</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2013-801-166</t>
+          <t>2013-801-028</t>
         </is>
       </c>
       <c r="E76" s="2" t="n">
-        <v>42781</v>
+        <v>41565</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Resolución de conflictos societarios</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>2013-01-408823</t>
         </is>
       </c>
     </row>
@@ -2428,20 +2808,25 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Nulidad de los actos defraudatorios</t>
+          <t>Régimen de conflicto de intereses</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2015-800-266</t>
+          <t>2018-800-00409</t>
         </is>
       </c>
       <c r="E77" s="2" t="n">
-        <v>42579</v>
+        <v>43677</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Nulidad de los actos defraudatorios</t>
+          <t>Régimen de conflicto de intereses</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>2019-01-292573</t>
         </is>
       </c>
     </row>
@@ -2454,20 +2839,25 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
+          <t>Impugnación de actos de asambleas, juntas directivas, juntas de socios o de cualquier otro órgano directivo de personas sometidas a su supervisión. Código General del Proceso artículo 24 numeral quinto letra c)</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2015-800-182</t>
+          <t>2015-800-165</t>
         </is>
       </c>
       <c r="E78" s="2" t="n">
-        <v>42619</v>
+        <v>42488</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
+          <t>Impugnación de decisiones sociales</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>2016-01-238418</t>
         </is>
       </c>
     </row>
@@ -2480,20 +2870,25 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2015-800-32</t>
+          <t>2022-800-00365</t>
         </is>
       </c>
       <c r="E79" s="2" t="n">
-        <v>42762</v>
+        <v>45153</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>2023-01-650584</t>
         </is>
       </c>
     </row>
@@ -2506,20 +2901,25 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Responsabilidad de liquidadores</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2017-800-00282</t>
+          <t>2017-800-00150</t>
         </is>
       </c>
       <c r="E80" s="2" t="n">
-        <v>43438</v>
+        <v>43032</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Responsabilidad de liquidadores</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>2017-01-545720</t>
         </is>
       </c>
     </row>
@@ -2532,20 +2932,25 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2017-800-00256</t>
+          <t>2022-800-00434</t>
         </is>
       </c>
       <c r="E81" s="2" t="n">
-        <v>43489</v>
+        <v>45196</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>2023-01-779371</t>
         </is>
       </c>
     </row>
@@ -2563,15 +2968,20 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2022-800-00215</t>
+          <t>2016-800-9</t>
         </is>
       </c>
       <c r="E82" s="2" t="n">
-        <v>44999</v>
+        <v>42528</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
           <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>2016-01-309133</t>
         </is>
       </c>
     </row>
@@ -2589,15 +2999,20 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2014801013</t>
+          <t>2019-800-00033</t>
         </is>
       </c>
       <c r="E83" s="2" t="n">
-        <v>41754</v>
+        <v>43900</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
           <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>2020-01-101271</t>
         </is>
       </c>
     </row>
@@ -2610,20 +3025,25 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Impugnación de actos de asambleas, juntas directivas, juntas de socios o de cualquier otro órgano directivo de personas sometidas a su supervisión. Código General del Proceso artículo 24 numeral quinto letra c)</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2018-800-00396</t>
+          <t>2014-801-158</t>
         </is>
       </c>
       <c r="E84" s="2" t="n">
-        <v>43626</v>
+        <v>42179</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Impugnación de decisiones sociales</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>2015-01-286125</t>
         </is>
       </c>
     </row>
@@ -2636,20 +3056,25 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Impugnación de actos de asambleas, juntas directivas, juntas de socios o de cualquier otro órgano directivo de personas sometidas a su supervisión. Código General del Proceso artículo 24 numeral quinto letra c)</t>
+          <t>Abuso del derecho de voto</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2016-800-196</t>
+          <t>2014-801-166</t>
         </is>
       </c>
       <c r="E85" s="2" t="n">
-        <v>42907</v>
+        <v>42139</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Impugnación de decisiones sociales</t>
+          <t>Abuso del derecho de voto</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>2015-01-246390</t>
         </is>
       </c>
     </row>
@@ -2662,20 +3087,25 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Impugnación de actos de asambleas, juntas directivas, juntas de socios o de cualquier otro órgano directivo de personas sometidas a su supervisión. Código General del Proceso artículo 24 numeral quinto letra c)</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>800-000034</t>
+          <t>810-000053</t>
         </is>
       </c>
       <c r="E86" s="2" t="n">
-        <v>41137</v>
+        <v>42137</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Impugnación de decisiones sociales</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>2015-01-243933</t>
         </is>
       </c>
     </row>
@@ -2704,6 +3134,11 @@
           <t>Responsabilidad de liquidadores</t>
         </is>
       </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>2022-01-048378</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -2726,6 +3161,11 @@
         <v>42362</v>
       </c>
       <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>2015-01-525152</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -2748,6 +3188,11 @@
         <v>43369</v>
       </c>
       <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>2018-01-423660</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -2766,6 +3211,11 @@
         <v>43360</v>
       </c>
       <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>2018-01-411664</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -2788,6 +3238,11 @@
         <v>43521</v>
       </c>
       <c r="F91" t="inlineStr"/>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>2019-01-042026</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -2814,6 +3269,11 @@
           <t>Responsabilidad de liquidadores</t>
         </is>
       </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>2017-01-206931</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -2840,6 +3300,11 @@
           <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>2017-01-346314</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -2866,6 +3331,11 @@
           <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>2017-01-361172</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -2892,6 +3362,11 @@
           <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>2017-01-632705</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -2918,6 +3393,11 @@
           <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>2018-01-006530</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -2944,6 +3424,11 @@
           <t>Enajenación de acciones</t>
         </is>
       </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>2018-01-542252</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -2966,6 +3451,11 @@
         <v>44970</v>
       </c>
       <c r="F98" t="inlineStr"/>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>2023-01-073689</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -2992,6 +3482,11 @@
           <t>Responsabilidad de liquidadores</t>
         </is>
       </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>2016-01-349290</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -3018,6 +3513,11 @@
           <t>Abuso del derecho de voto</t>
         </is>
       </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>2017-01-013829</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -3044,6 +3544,11 @@
           <t>Resolución de conflictos societarios</t>
         </is>
       </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>2019-01-317862</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -3070,6 +3575,11 @@
           <t>Responsabilidad de liquidadores</t>
         </is>
       </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>2018-01-300519</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -3096,6 +3606,11 @@
           <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>2022-01-533469</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -3122,6 +3637,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>2024-01-083355</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -3148,6 +3668,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>2023-01-654243</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -3174,6 +3699,11 @@
           <t>Reconocimiento de presupuestos de ineficacia</t>
         </is>
       </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>2020-01-270914</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -3200,6 +3730,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>2015-01-280201</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -3226,6 +3761,11 @@
           <t>Designación de peritos</t>
         </is>
       </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>2015-01-362534</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -3252,6 +3792,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>2015-01-368105</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -3278,6 +3823,11 @@
           <t>Régimen de conflicto de intereses</t>
         </is>
       </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>2017-01-529992</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -3304,6 +3854,11 @@
           <t>Responsabilidad de liquidadores</t>
         </is>
       </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>2017-01-638098</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -3330,6 +3885,11 @@
           <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>2016-01-500948</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -3356,6 +3916,11 @@
           <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>2019-01-383901</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -3382,6 +3947,11 @@
           <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>2024-01-592471</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -3408,6 +3978,11 @@
           <t>Abuso del derecho de voto</t>
         </is>
       </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>2018-01-428385</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -3434,6 +4009,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>2019-01-352235</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -3444,20 +4024,25 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>2017-800-70</t>
+          <t>2017-800-00158</t>
         </is>
       </c>
       <c r="E117" s="2" t="n">
-        <v>43200</v>
+        <v>43318</v>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>2018-01-360173</t>
         </is>
       </c>
     </row>
@@ -3470,20 +4055,25 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>2013-801-059</t>
+          <t>2017-800-00234</t>
         </is>
       </c>
       <c r="E118" s="2" t="n">
-        <v>41514</v>
+        <v>43119</v>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>2018-01-013074</t>
         </is>
       </c>
     </row>
@@ -3496,20 +4086,25 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Designación de peritos</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>801-000042</t>
+          <t>2015-800-34</t>
         </is>
       </c>
       <c r="E119" s="2" t="n">
-        <v>41474</v>
+        <v>43161</v>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Designación de peritos</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>2018-01-076748</t>
         </is>
       </c>
     </row>
@@ -3522,20 +4117,25 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Resolución de conflictos societarios</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>2014-801-177</t>
+          <t>2015-800-303</t>
         </is>
       </c>
       <c r="E120" s="2" t="n">
-        <v>42121</v>
+        <v>42863</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Resolución de conflictos societarios</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>2017-01-246764</t>
         </is>
       </c>
     </row>
@@ -3548,20 +4148,25 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Resolución de conflictos societarios</t>
+          <t>Diferencias que ocurran entre los accionistas, o entre éstos y la sociedad o entre éstos y sus administradores, en desarrollo del contrato social o del acto unilateral. Código General del Proceso artículo 24 numeral quinta letra b)</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>2013-802-019</t>
+          <t>2016-800-171</t>
         </is>
       </c>
       <c r="E121" s="2" t="n">
-        <v>42360</v>
+        <v>42690</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Resolución de conflictos societarios</t>
+          <t>Inexistencia de las decisiones sociales</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>2016-01-551771</t>
         </is>
       </c>
     </row>
@@ -3590,6 +4195,11 @@
           <t>Resolución de conflictos societarios</t>
         </is>
       </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>2016-01-311630</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -3616,6 +4226,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>2016-01-363230</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -3642,6 +4257,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>2016-01-522984</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -3668,6 +4288,11 @@
           <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>2016-01-500948</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -3694,6 +4319,11 @@
           <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>2019-01-383901</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -3704,20 +4334,25 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Impugnación de decisiones sociales</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>2019-800-00293</t>
+          <t>2014-801-263</t>
         </is>
       </c>
       <c r="E127" s="2" t="n">
-        <v>45469</v>
+        <v>42552</v>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>Impugnación de decisiones sociales</t>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>2016-01-363230</t>
         </is>
       </c>
     </row>
@@ -3730,20 +4365,25 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>2016-800-370</t>
+          <t>2015-800-25</t>
         </is>
       </c>
       <c r="E128" s="2" t="n">
-        <v>43370</v>
+        <v>42667</v>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>Abuso del derecho de voto</t>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>2016-01-522984</t>
         </is>
       </c>
     </row>
@@ -3756,20 +4396,25 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Enajenación de acciones</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>2018-800-00270</t>
+          <t>2013-801-123</t>
         </is>
       </c>
       <c r="E129" s="2" t="n">
-        <v>43735</v>
+        <v>41914</v>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Enajenación de acciones</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>2014-01-449616</t>
         </is>
       </c>
     </row>
@@ -3782,20 +4427,25 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Abuso del derecho de voto</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>2018-800-00361</t>
+          <t>2013801052</t>
         </is>
       </c>
       <c r="E130" s="2" t="n">
-        <v>43747</v>
+        <v>41627</v>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Abuso del derecho de voto</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>2013-01-546533</t>
         </is>
       </c>
     </row>
@@ -3808,20 +4458,25 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>2020-800-00031</t>
+          <t>2017-800-70</t>
         </is>
       </c>
       <c r="E131" s="2" t="n">
-        <v>44433</v>
+        <v>43200</v>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>2018-01-141081</t>
         </is>
       </c>
     </row>
@@ -3850,6 +4505,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>2018-01-341100</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -3876,6 +4536,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>2024-01-540244</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -3902,6 +4567,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>2012-01-411897</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -3928,6 +4598,11 @@
           <t>Responsabilidad de los administradores</t>
         </is>
       </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>2018-01-345453</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -3954,6 +4629,11 @@
           <t>Abuso del derecho de voto</t>
         </is>
       </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>2016-01-076363</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -3964,20 +4644,25 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>810-000057</t>
+          <t>2015-800-88</t>
         </is>
       </c>
       <c r="E137" s="2" t="n">
-        <v>43290</v>
+        <v>42277</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Responsabilidad de los administradores</t>
+          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>2015-01-398811</t>
         </is>
       </c>
     </row>
@@ -3990,20 +4675,25 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Enajenación de acciones</t>
+          <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>2018-800-00221</t>
+          <t>2016-800-318</t>
         </is>
       </c>
       <c r="E138" s="2" t="n">
-        <v>43679</v>
+        <v>43293</v>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>Enajenación de acciones</t>
+          <t>Desestimación de la personalidad jurídica</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>2018-01-320178</t>
         </is>
       </c>
     </row>
@@ -4016,20 +4706,25 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>2015-800-130</t>
+          <t>2015-800-267</t>
         </is>
       </c>
       <c r="E139" s="2" t="n">
-        <v>42394</v>
+        <v>42958</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>Discrepancias sobre el acaecimiento de causales de disolución</t>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>2017-01-426087</t>
         </is>
       </c>
     </row>
@@ -4042,20 +4737,25 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Impugnación de decisiones sociales</t>
+          <t>Reconocimiento de los presupuestos de ineficacia previstos en el Libro Segundo del Código de Comercio. Ley 446 de 1998 artículo 133, actualmente incorporado al Estatuto Orgánico del Sistema Financiero en su artículo 326 numeral octavo</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>2016-800-144</t>
+          <t>2016-800-069</t>
         </is>
       </c>
       <c r="E140" s="2" t="n">
-        <v>42611</v>
+        <v>42816</v>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>Impugnación de decisiones sociales</t>
+          <t>Reconocimiento de presupuestos de ineficacia</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>2017-01-121577</t>
         </is>
       </c>
     </row>
@@ -4068,20 +4768,25 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Responsabilidad de los administradores</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>2015-801-4</t>
+          <t>2017-800-00248</t>
         </is>
       </c>
       <c r="E141" s="2" t="n">
-        <v>42135</v>
+        <v>43521</v>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>Desestimación de la personalidad jurídica</t>
+          <t>Responsabilidad de los administradores</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>2019-01-042088</t>
         </is>
       </c>
     </row>
@@ -4110,6 +4815,11 @@
           <t>Resolución de conflictos societarios</t>
         </is>
       </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>2019-01-183815</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -4136,6 +4846,11 @@
           <t>Abuso del derecho de voto</t>
         </is>
       </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>2019-01-352247</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -4162,6 +4877,11 @@
           <t>Inexistencia de las decisiones sociales</t>
         </is>
       </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>2019-01-181262</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -4188,6 +4908,11 @@
           <t>Desestimación de la personalidad jurídica</t>
         </is>
       </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>2017-01-339746</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -4214,6 +4939,11 @@
           <t>Régimen de conflicto de intereses</t>
         </is>
       </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>2017-01-410118</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -4240,6 +4970,11 @@
           <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>2017-01-320607</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -4266,6 +5001,11 @@
           <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>2014-01-438835</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -4292,6 +5032,11 @@
           <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>2013-01-510035</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -4318,6 +5063,11 @@
           <t>Impugnación de decisiones sociales</t>
         </is>
       </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>2012-01-217776</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -4342,6 +5092,11 @@
       <c r="F151" t="inlineStr">
         <is>
           <t>Impugnación de decisiones sociales</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>2014-01-315639</t>
         </is>
       </c>
     </row>

</xml_diff>